<commit_message>
fix the Canadian Basin
</commit_message>
<xml_diff>
--- a/County_Basin_IDs.xlsx
+++ b/County_Basin_IDs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adel\Documents\GitHub\TWDB_script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{299DBE92-4469-43E1-8992-09EEBCFF84C1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59201F6-B5E3-412F-8678-4DC104BC707F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10005" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="County_FIPS" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="343">
   <si>
     <t>TX</t>
   </si>
@@ -1950,16 +1950,16 @@
       <selection activeCell="G221" sqref="G221"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1976,7 +1976,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1993,7 +1993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2010,7 +2010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -2027,7 +2027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -2044,7 +2044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -2078,7 +2078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -2095,7 +2095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -2112,7 +2112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -2129,7 +2129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -2163,7 +2163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -2180,7 +2180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -2197,7 +2197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -2214,7 +2214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -2265,7 +2265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -2282,7 +2282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -2299,7 +2299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -2316,7 +2316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -2333,7 +2333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -2350,7 +2350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -2367,7 +2367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -2384,7 +2384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -2418,7 +2418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -2435,7 +2435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -2452,7 +2452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -2469,7 +2469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -2486,7 +2486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>0</v>
       </c>
@@ -2503,7 +2503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -2520,7 +2520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>0</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>0</v>
       </c>
@@ -2554,7 +2554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>0</v>
       </c>
@@ -2571,7 +2571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>0</v>
       </c>
@@ -2588,7 +2588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>0</v>
       </c>
@@ -2605,7 +2605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>0</v>
       </c>
@@ -2622,7 +2622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>0</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>0</v>
       </c>
@@ -2656,7 +2656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>0</v>
       </c>
@@ -2673,7 +2673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>0</v>
       </c>
@@ -2690,7 +2690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>0</v>
       </c>
@@ -2707,7 +2707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>0</v>
       </c>
@@ -2724,7 +2724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>0</v>
       </c>
@@ -2741,7 +2741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>0</v>
       </c>
@@ -2758,7 +2758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>0</v>
       </c>
@@ -2775,7 +2775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>0</v>
       </c>
@@ -2792,7 +2792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>0</v>
       </c>
@@ -2809,7 +2809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>0</v>
       </c>
@@ -2826,7 +2826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>0</v>
       </c>
@@ -2843,7 +2843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>0</v>
       </c>
@@ -2860,7 +2860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>0</v>
       </c>
@@ -2877,7 +2877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>0</v>
       </c>
@@ -2894,7 +2894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>0</v>
       </c>
@@ -2911,7 +2911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>0</v>
       </c>
@@ -2928,7 +2928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>0</v>
       </c>
@@ -2945,7 +2945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>0</v>
       </c>
@@ -2962,7 +2962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>0</v>
       </c>
@@ -2979,7 +2979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>0</v>
       </c>
@@ -2996,7 +2996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>0</v>
       </c>
@@ -3013,7 +3013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>0</v>
       </c>
@@ -3030,7 +3030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>0</v>
       </c>
@@ -3047,7 +3047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>0</v>
       </c>
@@ -3064,7 +3064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>0</v>
       </c>
@@ -3081,7 +3081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>0</v>
       </c>
@@ -3098,7 +3098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>0</v>
       </c>
@@ -3115,7 +3115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>0</v>
       </c>
@@ -3132,7 +3132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>0</v>
       </c>
@@ -3149,7 +3149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>0</v>
       </c>
@@ -3166,7 +3166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>0</v>
       </c>
@@ -3183,7 +3183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>0</v>
       </c>
@@ -3200,7 +3200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>0</v>
       </c>
@@ -3217,7 +3217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>0</v>
       </c>
@@ -3234,7 +3234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>0</v>
       </c>
@@ -3251,7 +3251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>0</v>
       </c>
@@ -3268,7 +3268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>0</v>
       </c>
@@ -3285,7 +3285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>0</v>
       </c>
@@ -3302,7 +3302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>0</v>
       </c>
@@ -3319,7 +3319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>0</v>
       </c>
@@ -3336,7 +3336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>0</v>
       </c>
@@ -3353,7 +3353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>0</v>
       </c>
@@ -3370,7 +3370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>0</v>
       </c>
@@ -3387,7 +3387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>0</v>
       </c>
@@ -3404,7 +3404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>0</v>
       </c>
@@ -3421,7 +3421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>0</v>
       </c>
@@ -3438,7 +3438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>0</v>
       </c>
@@ -3455,7 +3455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>0</v>
       </c>
@@ -3472,7 +3472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>0</v>
       </c>
@@ -3489,7 +3489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>0</v>
       </c>
@@ -3506,7 +3506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>0</v>
       </c>
@@ -3523,7 +3523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>0</v>
       </c>
@@ -3540,7 +3540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>0</v>
       </c>
@@ -3557,7 +3557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>0</v>
       </c>
@@ -3574,7 +3574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>0</v>
       </c>
@@ -3591,7 +3591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>0</v>
       </c>
@@ -3608,7 +3608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>0</v>
       </c>
@@ -3625,7 +3625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>0</v>
       </c>
@@ -3642,7 +3642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>0</v>
       </c>
@@ -3659,7 +3659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>0</v>
       </c>
@@ -3676,7 +3676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>0</v>
       </c>
@@ -3693,7 +3693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>0</v>
       </c>
@@ -3710,7 +3710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>0</v>
       </c>
@@ -3727,7 +3727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>0</v>
       </c>
@@ -3744,7 +3744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>0</v>
       </c>
@@ -3761,7 +3761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>0</v>
       </c>
@@ -3778,7 +3778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>0</v>
       </c>
@@ -3795,7 +3795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>0</v>
       </c>
@@ -3812,7 +3812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>0</v>
       </c>
@@ -3829,7 +3829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>0</v>
       </c>
@@ -3846,7 +3846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>0</v>
       </c>
@@ -3863,7 +3863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>0</v>
       </c>
@@ -3880,7 +3880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>0</v>
       </c>
@@ -3897,7 +3897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>0</v>
       </c>
@@ -3914,7 +3914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>0</v>
       </c>
@@ -3931,7 +3931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>0</v>
       </c>
@@ -3948,7 +3948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>0</v>
       </c>
@@ -3965,7 +3965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>0</v>
       </c>
@@ -3982,7 +3982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>0</v>
       </c>
@@ -3999,7 +3999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>0</v>
       </c>
@@ -4016,7 +4016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>0</v>
       </c>
@@ -4033,7 +4033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>0</v>
       </c>
@@ -4050,7 +4050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>0</v>
       </c>
@@ -4067,7 +4067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>0</v>
       </c>
@@ -4084,7 +4084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>0</v>
       </c>
@@ -4101,7 +4101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>0</v>
       </c>
@@ -4118,7 +4118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>0</v>
       </c>
@@ -4135,7 +4135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>0</v>
       </c>
@@ -4152,7 +4152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>0</v>
       </c>
@@ -4169,7 +4169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>0</v>
       </c>
@@ -4186,7 +4186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>0</v>
       </c>
@@ -4203,7 +4203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>0</v>
       </c>
@@ -4220,7 +4220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>0</v>
       </c>
@@ -4237,7 +4237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>0</v>
       </c>
@@ -4254,7 +4254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>0</v>
       </c>
@@ -4271,7 +4271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>0</v>
       </c>
@@ -4288,7 +4288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>0</v>
       </c>
@@ -4305,7 +4305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>0</v>
       </c>
@@ -4322,7 +4322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>0</v>
       </c>
@@ -4339,7 +4339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>0</v>
       </c>
@@ -4356,7 +4356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>0</v>
       </c>
@@ -4373,7 +4373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>0</v>
       </c>
@@ -4390,7 +4390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>0</v>
       </c>
@@ -4407,7 +4407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>0</v>
       </c>
@@ -4424,7 +4424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>0</v>
       </c>
@@ -4441,7 +4441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>0</v>
       </c>
@@ -4458,7 +4458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>0</v>
       </c>
@@ -4475,7 +4475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>0</v>
       </c>
@@ -4492,7 +4492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>0</v>
       </c>
@@ -4509,7 +4509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>0</v>
       </c>
@@ -4526,7 +4526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>0</v>
       </c>
@@ -4543,7 +4543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>0</v>
       </c>
@@ -4560,7 +4560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>0</v>
       </c>
@@ -4577,7 +4577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>0</v>
       </c>
@@ -4594,7 +4594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>0</v>
       </c>
@@ -4611,7 +4611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>0</v>
       </c>
@@ -4628,7 +4628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>0</v>
       </c>
@@ -4645,7 +4645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>0</v>
       </c>
@@ -4662,7 +4662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>0</v>
       </c>
@@ -4679,7 +4679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>0</v>
       </c>
@@ -4696,7 +4696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>0</v>
       </c>
@@ -4713,7 +4713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>0</v>
       </c>
@@ -4730,7 +4730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>0</v>
       </c>
@@ -4747,7 +4747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>0</v>
       </c>
@@ -4764,7 +4764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>0</v>
       </c>
@@ -4781,7 +4781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>0</v>
       </c>
@@ -4798,7 +4798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>0</v>
       </c>
@@ -4815,7 +4815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>0</v>
       </c>
@@ -4832,7 +4832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>0</v>
       </c>
@@ -4849,7 +4849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>0</v>
       </c>
@@ -4866,7 +4866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>0</v>
       </c>
@@ -4883,7 +4883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>0</v>
       </c>
@@ -4900,7 +4900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>0</v>
       </c>
@@ -4917,7 +4917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>0</v>
       </c>
@@ -4934,7 +4934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>0</v>
       </c>
@@ -4951,7 +4951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>0</v>
       </c>
@@ -4968,7 +4968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>0</v>
       </c>
@@ -4985,7 +4985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>0</v>
       </c>
@@ -5002,7 +5002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>0</v>
       </c>
@@ -5019,7 +5019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>0</v>
       </c>
@@ -5036,7 +5036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>0</v>
       </c>
@@ -5053,7 +5053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>0</v>
       </c>
@@ -5070,7 +5070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>0</v>
       </c>
@@ -5087,7 +5087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>0</v>
       </c>
@@ -5104,7 +5104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>0</v>
       </c>
@@ -5121,7 +5121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>0</v>
       </c>
@@ -5138,7 +5138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>0</v>
       </c>
@@ -5155,7 +5155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>0</v>
       </c>
@@ -5172,7 +5172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>0</v>
       </c>
@@ -5189,7 +5189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>0</v>
       </c>
@@ -5206,7 +5206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>0</v>
       </c>
@@ -5223,7 +5223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>0</v>
       </c>
@@ -5240,7 +5240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>0</v>
       </c>
@@ -5257,7 +5257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>0</v>
       </c>
@@ -5274,7 +5274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>0</v>
       </c>
@@ -5291,7 +5291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>0</v>
       </c>
@@ -5308,7 +5308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>0</v>
       </c>
@@ -5325,7 +5325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>0</v>
       </c>
@@ -5342,7 +5342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>0</v>
       </c>
@@ -5359,7 +5359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>0</v>
       </c>
@@ -5376,7 +5376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>0</v>
       </c>
@@ -5393,7 +5393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>0</v>
       </c>
@@ -5410,7 +5410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>0</v>
       </c>
@@ -5427,7 +5427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>0</v>
       </c>
@@ -5444,7 +5444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>0</v>
       </c>
@@ -5461,7 +5461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>0</v>
       </c>
@@ -5478,7 +5478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>0</v>
       </c>
@@ -5495,7 +5495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>0</v>
       </c>
@@ -5512,7 +5512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>0</v>
       </c>
@@ -5529,7 +5529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>0</v>
       </c>
@@ -5546,7 +5546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>0</v>
       </c>
@@ -5563,7 +5563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>0</v>
       </c>
@@ -5580,7 +5580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>0</v>
       </c>
@@ -5597,7 +5597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>0</v>
       </c>
@@ -5614,7 +5614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
         <v>0</v>
       </c>
@@ -5631,7 +5631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>0</v>
       </c>
@@ -5648,7 +5648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
         <v>0</v>
       </c>
@@ -5665,7 +5665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
         <v>0</v>
       </c>
@@ -5682,7 +5682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
         <v>0</v>
       </c>
@@ -5699,7 +5699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>0</v>
       </c>
@@ -5716,7 +5716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>0</v>
       </c>
@@ -5733,7 +5733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>0</v>
       </c>
@@ -5750,7 +5750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>0</v>
       </c>
@@ -5767,7 +5767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
         <v>0</v>
       </c>
@@ -5784,7 +5784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>0</v>
       </c>
@@ -5801,7 +5801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
         <v>0</v>
       </c>
@@ -5818,7 +5818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
         <v>0</v>
       </c>
@@ -5835,7 +5835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
         <v>0</v>
       </c>
@@ -5852,7 +5852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
         <v>0</v>
       </c>
@@ -5869,7 +5869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
         <v>0</v>
       </c>
@@ -5886,7 +5886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
         <v>0</v>
       </c>
@@ -5903,7 +5903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
         <v>0</v>
       </c>
@@ -5920,7 +5920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
         <v>0</v>
       </c>
@@ -5937,7 +5937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
         <v>0</v>
       </c>
@@ -5954,7 +5954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
         <v>0</v>
       </c>
@@ -5971,7 +5971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
         <v>0</v>
       </c>
@@ -5988,7 +5988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
         <v>0</v>
       </c>
@@ -6005,7 +6005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
         <v>0</v>
       </c>
@@ -6022,7 +6022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
         <v>0</v>
       </c>
@@ -6039,7 +6039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
         <v>0</v>
       </c>
@@ -6056,7 +6056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
         <v>0</v>
       </c>
@@ -6073,7 +6073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
         <v>0</v>
       </c>
@@ -6090,7 +6090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
         <v>0</v>
       </c>
@@ -6107,7 +6107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
         <v>0</v>
       </c>
@@ -6124,7 +6124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
         <v>0</v>
       </c>
@@ -6141,7 +6141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
         <v>0</v>
       </c>
@@ -6158,7 +6158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
         <v>0</v>
       </c>
@@ -6175,7 +6175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
         <v>0</v>
       </c>
@@ -6192,7 +6192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
         <v>0</v>
       </c>
@@ -6209,7 +6209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
         <v>0</v>
       </c>
@@ -6226,7 +6226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
         <v>0</v>
       </c>
@@ -6243,7 +6243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
         <v>0</v>
       </c>
@@ -6260,7 +6260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
         <v>0</v>
       </c>
@@ -6277,7 +6277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
         <v>0</v>
       </c>
@@ -6305,19 +6305,19 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="19.26953125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7265625" customWidth="1"/>
+    <col min="5" max="5" width="8.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -6334,7 +6334,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -6351,7 +6351,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -6368,7 +6368,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -6385,7 +6385,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -6402,7 +6402,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -6419,7 +6419,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -6436,7 +6436,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -6453,7 +6453,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -6470,7 +6470,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -6487,7 +6487,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -6504,7 +6504,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -6521,7 +6521,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -6538,7 +6538,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -6555,7 +6555,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -6572,7 +6572,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -6589,7 +6589,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -6606,7 +6606,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -6623,7 +6623,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -6640,7 +6640,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -6657,7 +6657,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -6674,7 +6674,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -6691,7 +6691,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -6708,12 +6708,21 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
       <c r="B24" s="4">
-        <v>9999</v>
+        <v>1</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>342</v>
+      </c>
+      <c r="D24" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -6730,15 +6739,15 @@
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" customWidth="1"/>
-    <col min="4" max="4" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.54296875" customWidth="1"/>
+    <col min="4" max="4" width="27.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>36</v>
       </c>
@@ -6755,7 +6764,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -6772,7 +6781,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -6789,7 +6798,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -6806,7 +6815,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -6823,7 +6832,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -6840,7 +6849,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -6857,7 +6866,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -6874,7 +6883,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -6891,7 +6900,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -6908,7 +6917,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -6925,7 +6934,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -6942,7 +6951,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -6959,7 +6968,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -6976,7 +6985,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -6993,7 +7002,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -7010,7 +7019,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -7027,7 +7036,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -7044,7 +7053,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
         <v>18</v>
       </c>

</xml_diff>